<commit_message>
Add GPU models description
</commit_message>
<xml_diff>
--- a/Tables/NERModelEvalResults.xlsx
+++ b/Tables/NERModelEvalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Documents\VŠE\DP\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFCE7F1-317F-4E3D-9B3D-6671400ABEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF69AAE5-2D45-4E84-A50C-61FA83719650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Evaluace NER modelů - porovnání</t>
+  </si>
+  <si>
+    <t>GPU_bert_cased</t>
   </si>
 </sst>
 </file>
@@ -354,8 +357,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -377,6 +381,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:H11"/>
+  <dimension ref="D2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,113 +680,122 @@
   <sheetData>
     <row r="2" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="2" t="s">
-        <v>4</v>
+      <c r="D9" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
GPU modely evaluace + doplneni konkretnich hodnot
</commit_message>
<xml_diff>
--- a/Tables/NERModelEvalResults.xlsx
+++ b/Tables/NERModelEvalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Documents\VŠE\DP\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF69AAE5-2D45-4E84-A50C-61FA83719650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABA66C6-77CA-43F2-8925-29DB5CAE82E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Model</t>
   </si>
@@ -75,28 +75,79 @@
     <t>65,70</t>
   </si>
   <si>
-    <t>41,40</t>
-  </si>
-  <si>
     <t>63,48</t>
   </si>
   <si>
-    <t>lemmatizer_accuracy [%]</t>
-  </si>
-  <si>
-    <t>ner presision [%]</t>
-  </si>
-  <si>
     <t>ner recall [%]</t>
   </si>
   <si>
-    <t>ner F1 [%]</t>
-  </si>
-  <si>
     <t>Evaluace NER modelů - porovnání</t>
   </si>
   <si>
     <t>GPU_bert_cased</t>
+  </si>
+  <si>
+    <t>92,39</t>
+  </si>
+  <si>
+    <t>79,08</t>
+  </si>
+  <si>
+    <t>79,53</t>
+  </si>
+  <si>
+    <t>79,30</t>
+  </si>
+  <si>
+    <t>lemmatizer accuracy [%]</t>
+  </si>
+  <si>
+    <t>94,43</t>
+  </si>
+  <si>
+    <t>78,76</t>
+  </si>
+  <si>
+    <t>82,89</t>
+  </si>
+  <si>
+    <t>80,77</t>
+  </si>
+  <si>
+    <t>86,82</t>
+  </si>
+  <si>
+    <t>66,39</t>
+  </si>
+  <si>
+    <t>66,28</t>
+  </si>
+  <si>
+    <t>66,34</t>
+  </si>
+  <si>
+    <t>93,96</t>
+  </si>
+  <si>
+    <t>77,47</t>
+  </si>
+  <si>
+    <t>81,12</t>
+  </si>
+  <si>
+    <t>79,25</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ner precision [%]</t>
+  </si>
+  <si>
+    <t>ner F1 score [%]</t>
+  </si>
+  <si>
+    <t>61,40</t>
   </si>
 </sst>
 </file>
@@ -120,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +184,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -357,9 +414,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -381,8 +437,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:H12"/>
+  <dimension ref="D2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,127 +742,170 @@
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="11" t="s">
+    <row r="2" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="H8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="15" t="s">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>21</v>
+      <c r="E9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>9</v>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>12</v>
-      </c>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="18"/>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="5" t="s">
+    <row r="12" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update streamlit CPU version
</commit_message>
<xml_diff>
--- a/Tables/NERModelEvalResults.xlsx
+++ b/Tables/NERModelEvalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Documents\VŠE\DP\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABA66C6-77CA-43F2-8925-29DB5CAE82E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D679EA-1B72-4A4D-BF01-D7817037FD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,9 @@
     <t>Model</t>
   </si>
   <si>
+    <t>ner recall</t>
+  </si>
+  <si>
     <t>CPU_coarse</t>
   </si>
   <si>
@@ -78,9 +81,6 @@
     <t>63,48</t>
   </si>
   <si>
-    <t>ner recall [%]</t>
-  </si>
-  <si>
     <t>Evaluace NER modelů - porovnání</t>
   </si>
   <si>
@@ -99,9 +99,6 @@
     <t>79,30</t>
   </si>
   <si>
-    <t>lemmatizer accuracy [%]</t>
-  </si>
-  <si>
     <t>94,43</t>
   </si>
   <si>
@@ -141,13 +138,16 @@
     <t>-</t>
   </si>
   <si>
-    <t>ner precision [%]</t>
-  </si>
-  <si>
-    <t>ner F1 score [%]</t>
-  </si>
-  <si>
     <t>61,40</t>
+  </si>
+  <si>
+    <t>lemmatizer accuracy</t>
+  </si>
+  <si>
+    <t>ner precision</t>
+  </si>
+  <si>
+    <t>ner F1 score</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="D2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,69 +761,69 @@
         <v>0</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" s="19"/>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D5" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
@@ -843,68 +843,68 @@
         <v>19</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>27</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>